<commit_message>
Posting second lecture and activity
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yotescollegeofidaho-my.sharepoint.com/personal/efriedlander_collegeofidaho_edu/Documents/Teaching/MAT212WI25/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{971B5267-4E0E-4BC5-857F-BC96FE3C8F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AE951CD1-6AEF-4AC6-A8F7-7F8291FDFB6D}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{CBC1235C-26E4-431A-B657-B0CECB191CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7A048193-8DD9-4626-B382-FF3F9272C9DA}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="195">
   <si>
     <t>dow</t>
   </si>
@@ -573,9 +573,6 @@
     <t>Final Poster Presentation</t>
   </si>
   <si>
-    <t>day</t>
-  </si>
-  <si>
     <t>Welcome to MAT 212</t>
   </si>
   <si>
@@ -585,9 +582,6 @@
     <t>Introduction to Simple Linear Regression</t>
   </si>
   <si>
-    <t>/prepare/prep-01.qmd</t>
-  </si>
-  <si>
     <t>/ae/ae-01-multivariate-relationships.qmd</t>
   </si>
   <si>
@@ -604,6 +598,27 @@
   </si>
   <si>
     <t>/project/project-instructions.qmd#project-proposal</t>
+  </si>
+  <si>
+    <t>lecture</t>
+  </si>
+  <si>
+    <t>/prepare/prep-02.qmd</t>
+  </si>
+  <si>
+    <t>/prepare/prep-03.qmd</t>
+  </si>
+  <si>
+    <t>Simulation-Based Inference</t>
+  </si>
+  <si>
+    <t>/ae/ae-02-bikeshare.qmd</t>
+  </si>
+  <si>
+    <t>/slides/02-slr-intro.qmd</t>
+  </si>
+  <si>
+    <t>F/M</t>
   </si>
 </sst>
 </file>
@@ -1150,10 +1165,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1473,10 +1484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C666FC1-734D-4F31-9D28-5509B94BC597}">
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1489,7 +1500,7 @@
         <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -1530,24 +1541,24 @@
         <v>1</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>12</v>
+        <v>194</v>
       </c>
       <c r="D2" s="6">
         <v>45660</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I2" s="17"/>
       <c r="J2" s="8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="K2" s="8"/>
       <c r="L2" s="5" t="s">
@@ -1568,279 +1579,284 @@
         <v>45663</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="G3" s="5"/>
+        <v>189</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="H3" t="s">
+        <v>192</v>
+      </c>
       <c r="I3" s="8"/>
       <c r="J3" s="8" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="K3" s="8"/>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="1:12" ht="66" x14ac:dyDescent="0.3">
-      <c r="B4" s="4"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="18" t="s">
+    <row r="4" spans="1:12" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="6">
+        <v>45663</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="5"/>
+    </row>
+    <row r="5" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+      <c r="B5" s="4"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8" t="s">
-        <v>187</v>
-      </c>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-    </row>
-    <row r="5" spans="1:12" ht="66" x14ac:dyDescent="0.3">
-      <c r="B5" s="10"/>
-      <c r="C5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="6">
-        <v>45532</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H5" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="17" t="s">
-        <v>19</v>
-      </c>
+      <c r="I5" s="8"/>
       <c r="J5" s="8" t="s">
-        <v>188</v>
-      </c>
-      <c r="K5" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="L5" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
+        <v>185</v>
+      </c>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+    </row>
+    <row r="6" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B6" s="10"/>
       <c r="C6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="6">
+        <v>45532</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B7" s="10"/>
+      <c r="C7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D7" s="6">
         <v>45534</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E7" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5" t="s">
+      <c r="F7" s="5"/>
+      <c r="G7" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H7" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="K6" s="27"/>
-      <c r="L6" s="12"/>
-    </row>
-    <row r="7" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B7" s="4">
+      <c r="I7" s="8"/>
+      <c r="J7" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="K7" s="27"/>
+      <c r="L7" s="12"/>
+    </row>
+    <row r="8" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B8" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D8" s="6">
         <v>45537</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E8" s="28" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="B8" s="4"/>
-      <c r="C8" s="5" t="s">
+    <row r="9" spans="1:12" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="B9" s="4"/>
+      <c r="C9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D9" s="6">
         <v>45539</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="F9" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H9" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I8" s="8" t="s">
+      <c r="I9" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="8"/>
-      <c r="K8" t="s">
+      <c r="J9" s="8"/>
+      <c r="K9" t="s">
         <v>51</v>
       </c>
-      <c r="L8" s="8"/>
-    </row>
-    <row r="9" spans="1:12" ht="181.5" x14ac:dyDescent="0.3">
-      <c r="B9" s="10"/>
-      <c r="C9" s="5" t="s">
+      <c r="L9" s="8"/>
+    </row>
+    <row r="10" spans="1:12" ht="181.5" x14ac:dyDescent="0.3">
+      <c r="B10" s="10"/>
+      <c r="C10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D10" s="6">
         <v>45541</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G10" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H10" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="I9" s="9"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="9" t="s">
+      <c r="I10" s="9"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="L10" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="B10" s="4">
+    <row r="11" spans="1:12" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="B11" s="4">
         <v>4</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C11" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D11" s="6">
         <v>45544</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G11" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="H10" s="13"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-    </row>
-    <row r="11" spans="1:12" ht="148.5" x14ac:dyDescent="0.3">
-      <c r="B11" s="10"/>
-      <c r="C11" s="5" t="s">
+      <c r="H11" s="13"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+      <c r="L11" s="8"/>
+    </row>
+    <row r="12" spans="1:12" ht="148.5" x14ac:dyDescent="0.3">
+      <c r="B12" s="10"/>
+      <c r="C12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D12" s="6">
         <v>45546</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E12" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="5" t="s">
+      <c r="F12" s="8"/>
+      <c r="G12" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H12" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="J11" s="8"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="8"/>
-    </row>
-    <row r="12" spans="1:12" ht="66" x14ac:dyDescent="0.3">
-      <c r="B12" s="4"/>
-      <c r="C12" s="5" t="s">
+      <c r="J12" s="8"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="8"/>
+    </row>
+    <row r="13" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+      <c r="B13" s="4"/>
+      <c r="C13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D13" s="6">
         <v>45548</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F13" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G13" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="I12" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="J12" s="8"/>
-      <c r="K12" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="L12" s="8"/>
-    </row>
-    <row r="13" spans="1:12" ht="99" x14ac:dyDescent="0.3">
-      <c r="B13" s="31">
-        <v>5</v>
-      </c>
-      <c r="C13" s="32" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="33">
-        <v>45551</v>
-      </c>
-      <c r="E13" s="39" t="s">
-        <v>77</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="I13" s="36"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="34"/>
-    </row>
-    <row r="14" spans="1:12" ht="66" x14ac:dyDescent="0.3">
-      <c r="B14" s="31"/>
+      <c r="I13" s="30" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" s="8"/>
+      <c r="K13" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="L13" s="8"/>
+    </row>
+    <row r="14" spans="1:12" ht="99" x14ac:dyDescent="0.3">
+      <c r="B14" s="31">
+        <v>5</v>
+      </c>
       <c r="C14" s="32" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D14" s="33">
-        <v>45553</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>62</v>
+        <v>45551</v>
+      </c>
+      <c r="E14" s="39" t="s">
+        <v>77</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>63</v>
@@ -1849,7 +1865,7 @@
         <v>64</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I14" s="36"/>
       <c r="J14" s="34"/>
@@ -1859,269 +1875,271 @@
     <row r="15" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B15" s="31"/>
       <c r="C15" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="33">
+        <v>45553</v>
+      </c>
+      <c r="E15" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="I15" s="36"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="34"/>
+    </row>
+    <row r="16" spans="1:12" ht="66" x14ac:dyDescent="0.3">
+      <c r="B16" s="31"/>
+      <c r="C16" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="33">
+      <c r="D16" s="33">
         <v>45555</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E16" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="F15" s="34" t="s">
+      <c r="F16" s="34" t="s">
         <v>70</v>
       </c>
-      <c r="G15" s="35" t="s">
+      <c r="G16" s="35" t="s">
         <v>72</v>
       </c>
-      <c r="H15" s="38" t="s">
+      <c r="H16" s="38" t="s">
         <v>74</v>
       </c>
-      <c r="I15" s="36" t="s">
+      <c r="I16" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="J15" s="34"/>
-      <c r="K15" s="35" t="s">
+      <c r="J16" s="34"/>
+      <c r="K16" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="L15" s="34"/>
-    </row>
-    <row r="16" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B16" s="31">
+      <c r="L16" s="34"/>
+    </row>
+    <row r="17" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B17" s="31">
         <v>6</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C17" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="33">
+      <c r="D17" s="33">
         <v>45558</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E17" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="F16" s="34" t="s">
+      <c r="F17" s="34" t="s">
         <v>78</v>
       </c>
-      <c r="G16" s="35"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="36"/>
-      <c r="J16" s="51" t="s">
+      <c r="G17" s="35"/>
+      <c r="H17" s="38"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="K16" s="35" t="s">
+      <c r="K17" s="35" t="s">
         <v>80</v>
       </c>
-      <c r="L16" s="34"/>
-    </row>
-    <row r="17" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="B17" s="31"/>
-      <c r="C17" s="32" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="33">
-        <v>45560</v>
-      </c>
-      <c r="E17" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="I17" s="36"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="35"/>
       <c r="L17" s="34"/>
     </row>
-    <row r="18" spans="2:12" ht="33" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
       <c r="B18" s="31"/>
       <c r="C18" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="33">
+        <v>45560</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="I18" s="36"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="34"/>
+    </row>
+    <row r="19" spans="2:12" ht="33" x14ac:dyDescent="0.3">
+      <c r="B19" s="31"/>
+      <c r="C19" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="D18" s="33">
+      <c r="D19" s="33">
         <v>45562</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E19" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="F18" s="34" t="s">
+      <c r="F19" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="G18" s="35" t="s">
+      <c r="G19" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="H18" s="38" t="s">
+      <c r="H19" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="I18" s="36" t="s">
+      <c r="I19" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="J18" s="34"/>
-      <c r="K18" s="23" t="s">
+      <c r="J19" s="34"/>
+      <c r="K19" s="23" t="s">
         <v>79</v>
       </c>
-      <c r="L18" s="34"/>
-    </row>
-    <row r="19" spans="2:12" ht="66" x14ac:dyDescent="0.3">
-      <c r="B19" s="4">
+      <c r="L19" s="34"/>
+    </row>
+    <row r="20" spans="2:12" ht="66" x14ac:dyDescent="0.3">
+      <c r="B20" s="4">
         <v>7</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C20" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="21">
+      <c r="D20" s="21">
         <v>45565</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E20" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="F19" s="43" t="s">
+      <c r="F20" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="G19" s="25" t="s">
+      <c r="G20" s="25" t="s">
         <v>81</v>
-      </c>
-      <c r="H19" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23"/>
-      <c r="L19" s="23"/>
-    </row>
-    <row r="20" spans="2:12" ht="66" x14ac:dyDescent="0.3">
-      <c r="B20" s="19"/>
-      <c r="C20" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="D20" s="22">
-        <v>45567</v>
-      </c>
-      <c r="E20" s="39" t="s">
-        <v>86</v>
-      </c>
-      <c r="F20" s="43" t="s">
-        <v>88</v>
-      </c>
-      <c r="G20" s="25" t="s">
-        <v>87</v>
       </c>
       <c r="H20" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="I20" s="24"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="24"/>
-      <c r="L20" s="24"/>
-    </row>
-    <row r="21" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B21" s="10"/>
-      <c r="C21" s="40" t="s">
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="L20" s="23"/>
+    </row>
+    <row r="21" spans="2:12" ht="66" x14ac:dyDescent="0.3">
+      <c r="B21" s="19"/>
+      <c r="C21" s="41" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="22">
+        <v>45567</v>
+      </c>
+      <c r="E21" s="39" t="s">
+        <v>86</v>
+      </c>
+      <c r="F21" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="H21" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
+      <c r="K21" s="24"/>
+      <c r="L21" s="24"/>
+    </row>
+    <row r="22" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B22" s="10"/>
+      <c r="C22" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="22">
+      <c r="D22" s="22">
         <v>45569</v>
       </c>
-      <c r="E21" s="42" t="s">
+      <c r="E22" s="42" t="s">
         <v>84</v>
       </c>
-      <c r="F21" s="44" t="s">
+      <c r="F22" s="44" t="s">
         <v>98</v>
       </c>
-      <c r="G21" s="25" t="s">
+      <c r="G22" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="H21" s="26" t="s">
+      <c r="H22" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="I21" s="9" t="s">
+      <c r="I22" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8" t="s">
+      <c r="J22" s="8"/>
+      <c r="K22" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="L21" s="8"/>
-    </row>
-    <row r="22" spans="2:12" ht="66" x14ac:dyDescent="0.3">
-      <c r="B22" s="4">
+      <c r="L22" s="8"/>
+    </row>
+    <row r="23" spans="2:12" ht="66" x14ac:dyDescent="0.3">
+      <c r="B23" s="4">
         <v>8</v>
       </c>
-      <c r="C22" s="45" t="s">
+      <c r="C23" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="D22" s="46">
+      <c r="D23" s="46">
         <v>45572</v>
       </c>
-      <c r="E22" s="42" t="s">
+      <c r="E23" s="42" t="s">
         <v>93</v>
       </c>
-      <c r="F22" s="44" t="s">
+      <c r="F23" s="44" t="s">
         <v>97</v>
       </c>
-      <c r="G22" s="25" t="s">
+      <c r="G23" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="H22" s="26" t="s">
+      <c r="H23" s="26" t="s">
         <v>100</v>
-      </c>
-      <c r="I22" s="9"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-    </row>
-    <row r="23" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B23" s="4"/>
-      <c r="C23" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="6">
-        <v>45574</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="F23" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="G23" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="H23" s="26" t="s">
-        <v>101</v>
       </c>
       <c r="I23" s="9"/>
       <c r="J23" s="8"/>
-      <c r="K23" s="5"/>
+      <c r="K23" s="8"/>
       <c r="L23" s="8"/>
     </row>
-    <row r="24" spans="2:12" ht="33" x14ac:dyDescent="0.3">
-      <c r="B24" s="10"/>
+    <row r="24" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B24" s="4"/>
       <c r="C24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="6">
+        <v>45574</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="F24" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="H24" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="I24" s="9"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="5"/>
+      <c r="L24" s="8"/>
+    </row>
+    <row r="25" spans="2:12" ht="33" x14ac:dyDescent="0.3">
+      <c r="B25" s="10"/>
+      <c r="C25" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D25" s="6">
         <v>45576</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E25" s="7" t="s">
         <v>25</v>
-      </c>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="L24" s="8"/>
-    </row>
-    <row r="25" spans="2:12" ht="66" x14ac:dyDescent="0.3">
-      <c r="B25" s="4">
-        <v>9</v>
-      </c>
-      <c r="C25" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="D25" s="6">
-        <v>45579</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>95</v>
       </c>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
@@ -2129,17 +2147,19 @@
       <c r="I25" s="8"/>
       <c r="J25" s="8"/>
       <c r="K25" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L25" s="8"/>
     </row>
     <row r="26" spans="2:12" ht="66" x14ac:dyDescent="0.3">
-      <c r="B26" s="10"/>
-      <c r="C26" s="9" t="s">
-        <v>10</v>
+      <c r="B26" s="4">
+        <v>9</v>
+      </c>
+      <c r="C26" s="37" t="s">
+        <v>13</v>
       </c>
       <c r="D26" s="6">
-        <v>45581</v>
+        <v>45579</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>95</v>
@@ -2149,175 +2169,167 @@
       <c r="H26" s="8"/>
       <c r="I26" s="8"/>
       <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
+      <c r="K26" s="8" t="s">
+        <v>96</v>
+      </c>
       <c r="L26" s="8"/>
     </row>
     <row r="27" spans="2:12" ht="66" x14ac:dyDescent="0.3">
-      <c r="B27" s="4"/>
-      <c r="C27" s="5" t="s">
-        <v>12</v>
+      <c r="B27" s="10"/>
+      <c r="C27" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="D27" s="6">
-        <v>45583</v>
+        <v>45581</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="13"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
       <c r="J27" s="8"/>
       <c r="K27" s="8"/>
       <c r="L27" s="8"/>
     </row>
-    <row r="28" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B28" s="4">
-        <v>10</v>
-      </c>
+    <row r="28" spans="2:12" ht="66" x14ac:dyDescent="0.3">
+      <c r="B28" s="4"/>
       <c r="C28" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D28" s="6">
-        <v>45586</v>
+        <v>45583</v>
       </c>
       <c r="E28" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="G28" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>105</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="9"/>
       <c r="I28" s="13"/>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
     </row>
-    <row r="29" spans="2:12" ht="66" x14ac:dyDescent="0.3">
-      <c r="B29" s="10"/>
-      <c r="C29" s="9" t="s">
+    <row r="29" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B29" s="4">
         <v>10</v>
       </c>
+      <c r="C29" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="D29" s="6">
-        <v>45588</v>
+        <v>45586</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="G29" s="25" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="I29" s="8"/>
+        <v>105</v>
+      </c>
+      <c r="I29" s="13"/>
       <c r="J29" s="8"/>
       <c r="K29" s="8"/>
-      <c r="L29" s="5" t="s">
+      <c r="L29" s="8"/>
+    </row>
+    <row r="30" spans="2:12" ht="66" x14ac:dyDescent="0.3">
+      <c r="B30" s="10"/>
+      <c r="C30" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30" s="6">
+        <v>45588</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="G30" s="25" t="s">
+        <v>107</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+      <c r="L30" s="5" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="2:12" ht="99" x14ac:dyDescent="0.3">
-      <c r="B30" s="4"/>
-      <c r="C30" s="5" t="s">
+    <row r="31" spans="2:12" ht="99" x14ac:dyDescent="0.3">
+      <c r="B31" s="4"/>
+      <c r="C31" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="6">
+      <c r="D31" s="6">
         <v>45590</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E31" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="F30" s="8"/>
-      <c r="G30" s="25" t="s">
+      <c r="F31" s="8"/>
+      <c r="G31" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="H30" s="9" t="s">
+      <c r="H31" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="I30" s="9" t="s">
+      <c r="I31" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8" t="s">
+      <c r="J31" s="8"/>
+      <c r="K31" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="L30" s="8"/>
-    </row>
-    <row r="31" spans="2:12" ht="66" x14ac:dyDescent="0.3">
-      <c r="B31" s="4">
+      <c r="L31" s="8"/>
+    </row>
+    <row r="32" spans="2:12" ht="66" x14ac:dyDescent="0.3">
+      <c r="B32" s="4">
         <v>11</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C32" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D32" s="6">
         <v>45593</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="E32" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="F31" s="5" t="s">
+      <c r="F32" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="G31" s="25" t="s">
+      <c r="G32" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="H31" s="9" t="s">
+      <c r="H32" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="8"/>
-    </row>
-    <row r="32" spans="2:12" ht="66" x14ac:dyDescent="0.3">
-      <c r="B32" s="10"/>
-      <c r="C32" s="9" t="s">
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+      <c r="L32" s="8"/>
+    </row>
+    <row r="33" spans="2:12" ht="66" x14ac:dyDescent="0.3">
+      <c r="B33" s="10"/>
+      <c r="C33" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D33" s="6">
         <v>45595</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="E33" s="7" t="s">
         <v>124</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="G32" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="I32" s="47"/>
-      <c r="J32" s="50" t="s">
-        <v>115</v>
-      </c>
-      <c r="K32" s="47" t="s">
-        <v>116</v>
-      </c>
-      <c r="L32" s="47"/>
-    </row>
-    <row r="33" spans="2:12" ht="99" x14ac:dyDescent="0.3">
-      <c r="B33" s="4"/>
-      <c r="C33" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D33" s="6">
-        <v>45597</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>132</v>
       </c>
       <c r="F33" s="5" t="s">
         <v>123</v>
@@ -2328,209 +2340,207 @@
       <c r="H33" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="I33" s="9" t="s">
+      <c r="I33" s="47"/>
+      <c r="J33" s="50" t="s">
+        <v>115</v>
+      </c>
+      <c r="K33" s="47" t="s">
+        <v>116</v>
+      </c>
+      <c r="L33" s="47"/>
+    </row>
+    <row r="34" spans="2:12" ht="99" x14ac:dyDescent="0.3">
+      <c r="B34" s="4"/>
+      <c r="C34" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="6">
+        <v>45597</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G34" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="I34" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="K33" s="50" t="s">
+      <c r="K34" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="L33" s="50"/>
-    </row>
-    <row r="34" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B34" s="4">
+      <c r="L34" s="50"/>
+    </row>
+    <row r="35" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B35" s="4">
         <v>12</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C35" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D35" s="6">
         <v>45600</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="E35" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="F34" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="G34" s="25" t="s">
-        <v>128</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="I34" s="49"/>
-      <c r="J34" s="48"/>
-      <c r="K34" s="49"/>
-      <c r="L34" s="48"/>
-    </row>
-    <row r="35" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="B35" s="10"/>
-      <c r="C35" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D35" s="6">
-        <v>45602</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>130</v>
       </c>
       <c r="F35" s="5" t="s">
         <v>127</v>
       </c>
       <c r="G35" s="25" t="s">
+        <v>128</v>
+      </c>
+      <c r="H35" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="I35" s="49"/>
+      <c r="J35" s="48"/>
+      <c r="K35" s="49"/>
+      <c r="L35" s="48"/>
+    </row>
+    <row r="36" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="B36" s="10"/>
+      <c r="C36" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D36" s="6">
+        <v>45602</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="G36" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="H35" s="9" t="s">
+      <c r="H36" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="I35" s="8"/>
-      <c r="J35" s="9"/>
-      <c r="K35" s="13"/>
-      <c r="L35" s="8"/>
-    </row>
-    <row r="36" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="B36" s="4"/>
-      <c r="C36" s="5" t="s">
+      <c r="I36" s="8"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="13"/>
+      <c r="L36" s="8"/>
+    </row>
+    <row r="37" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="B37" s="4"/>
+      <c r="C37" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D37" s="6">
         <v>45604</v>
       </c>
-      <c r="E36" s="7" t="s">
+      <c r="E37" s="7" t="s">
         <v>140</v>
       </c>
-      <c r="G36" s="25" t="s">
+      <c r="G37" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="H36" s="9" t="s">
+      <c r="H37" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="I36" s="9" t="s">
+      <c r="I37" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="J36" s="8"/>
-      <c r="K36" s="50" t="s">
+      <c r="J37" s="8"/>
+      <c r="K37" s="50" t="s">
         <v>133</v>
       </c>
-      <c r="L36" s="8"/>
-    </row>
-    <row r="37" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="B37" s="4">
+      <c r="L37" s="8"/>
+    </row>
+    <row r="38" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="B38" s="4">
         <v>13</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C38" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D38" s="6">
         <v>45607</v>
       </c>
-      <c r="E37" s="7" t="s">
+      <c r="E38" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="F37" s="5" t="s">
+      <c r="F38" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="G37" s="25" t="s">
+      <c r="G38" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="H37" s="9"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="5"/>
-      <c r="L37" s="8"/>
-    </row>
-    <row r="38" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="B38" s="10"/>
-      <c r="C38" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D38" s="6">
-        <v>45609</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F38" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="G38" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="H38" s="9" t="s">
-        <v>143</v>
-      </c>
+      <c r="H38" s="9"/>
       <c r="I38" s="8"/>
       <c r="J38" s="8"/>
-      <c r="K38" s="8"/>
+      <c r="K38" s="5"/>
       <c r="L38" s="8"/>
     </row>
-    <row r="39" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="B39" s="4"/>
+    <row r="39" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="B39" s="10"/>
       <c r="C39" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D39" s="6">
-        <v>45611</v>
+        <v>45609</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>149</v>
+        <v>30</v>
       </c>
       <c r="F39" s="5" t="s">
         <v>139</v>
       </c>
       <c r="G39" s="25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H39" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="I39" s="8"/>
       <c r="J39" s="8"/>
-      <c r="K39" s="8" t="s">
+      <c r="K39" s="8"/>
+      <c r="L39" s="8"/>
+    </row>
+    <row r="40" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="B40" s="4"/>
+      <c r="C40" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="6">
+        <v>45611</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="G40" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="H40" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="L39" s="8"/>
-    </row>
-    <row r="40" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="B40" s="4">
+      <c r="L40" s="8"/>
+    </row>
+    <row r="41" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="B41" s="4">
         <v>14</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C41" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D41" s="6">
         <v>45614</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>151</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="G40" s="25" t="s">
-        <v>153</v>
-      </c>
-      <c r="H40" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="I40" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="J40" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="K40" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="L40" s="8"/>
-    </row>
-    <row r="41" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="B41" s="10"/>
-      <c r="C41" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D41" s="6">
-        <v>45616</v>
       </c>
       <c r="E41" s="7" t="s">
         <v>151</v>
@@ -2544,18 +2554,24 @@
       <c r="H41" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="8"/>
-      <c r="L41" s="5"/>
+      <c r="I41" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="K41" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="L41" s="8"/>
     </row>
     <row r="42" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="B42" s="4"/>
-      <c r="C42" s="5" t="s">
-        <v>12</v>
+      <c r="B42" s="10"/>
+      <c r="C42" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="D42" s="6">
-        <v>45618</v>
+        <v>45616</v>
       </c>
       <c r="E42" s="7" t="s">
         <v>151</v>
@@ -2569,204 +2585,206 @@
       <c r="H42" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="I42" s="13"/>
+      <c r="I42" s="8"/>
       <c r="J42" s="8"/>
       <c r="K42" s="8"/>
-      <c r="L42" s="8"/>
-    </row>
-    <row r="43" spans="2:12" ht="33" x14ac:dyDescent="0.3">
-      <c r="B43" s="4">
+      <c r="L42" s="5"/>
+    </row>
+    <row r="43" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="B43" s="4"/>
+      <c r="C43" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43" s="6">
+        <v>45618</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="G43" s="25" t="s">
+        <v>153</v>
+      </c>
+      <c r="H43" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="I43" s="13"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+      <c r="L43" s="8"/>
+    </row>
+    <row r="44" spans="2:12" ht="33" x14ac:dyDescent="0.3">
+      <c r="B44" s="4">
         <v>15</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C44" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D44" s="6">
         <v>45621</v>
       </c>
-      <c r="E43" s="7" t="s">
+      <c r="E44" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="F43" s="8"/>
-      <c r="G43" s="25" t="s">
+      <c r="F44" s="8"/>
+      <c r="G44" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="H43" s="9" t="s">
+      <c r="H44" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="I43" s="13"/>
-      <c r="J43" s="8" t="s">
+      <c r="I44" s="13"/>
+      <c r="J44" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="K43" s="15" t="s">
+      <c r="K44" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="L43" s="8"/>
-    </row>
-    <row r="44" spans="2:12" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="B44" s="10"/>
-      <c r="C44" s="9" t="s">
+      <c r="L44" s="8"/>
+    </row>
+    <row r="45" spans="2:12" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="B45" s="10"/>
+      <c r="C45" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D44" s="6">
+      <c r="D45" s="6">
         <v>45623</v>
       </c>
-      <c r="E44" s="7" t="s">
+      <c r="E45" s="7" t="s">
         <v>161</v>
-      </c>
-      <c r="F44" s="8"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
-      <c r="J44" s="8"/>
-      <c r="K44" s="13"/>
-      <c r="L44" s="12"/>
-    </row>
-    <row r="45" spans="2:12" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="10"/>
-      <c r="C45" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D45" s="6">
-        <v>45625</v>
-      </c>
-      <c r="E45" s="11" t="s">
-        <v>32</v>
       </c>
       <c r="F45" s="8"/>
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
       <c r="I45" s="8"/>
       <c r="J45" s="8"/>
-      <c r="K45" s="8"/>
-      <c r="L45" s="8"/>
-    </row>
-    <row r="46" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="B46" s="4">
+      <c r="K45" s="13"/>
+      <c r="L45" s="12"/>
+    </row>
+    <row r="46" spans="2:12" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="10"/>
+      <c r="C46" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D46" s="6">
+        <v>45625</v>
+      </c>
+      <c r="E46" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F46" s="8"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
+      <c r="L46" s="8"/>
+    </row>
+    <row r="47" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
+      <c r="B47" s="4">
         <v>16</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C47" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D47" s="6">
         <v>45628</v>
       </c>
-      <c r="E46" s="7" t="s">
+      <c r="E47" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="F46" s="5" t="s">
+      <c r="F47" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="G46" s="25" t="s">
+      <c r="G47" s="25" t="s">
         <v>164</v>
       </c>
-      <c r="H46" s="9" t="s">
+      <c r="H47" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="I46" s="8"/>
-      <c r="K46" s="8"/>
-      <c r="L46" s="5"/>
-    </row>
-    <row r="47" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B47" s="10"/>
-      <c r="C47" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D47" s="6">
-        <v>45630</v>
-      </c>
-      <c r="E47" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="F47" s="8"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="13"/>
-      <c r="J47" s="8"/>
-      <c r="K47" s="5"/>
-      <c r="L47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="K47" s="8"/>
+      <c r="L47" s="5"/>
     </row>
     <row r="48" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B48" s="10"/>
-      <c r="C48" s="9" t="s">
-        <v>12</v>
+      <c r="C48" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="D48" s="6">
-        <v>45632</v>
+        <v>45630</v>
       </c>
       <c r="E48" s="7" t="s">
         <v>167</v>
       </c>
       <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="8"/>
-      <c r="I48" s="8" t="s">
-        <v>169</v>
-      </c>
+      <c r="G48" s="5"/>
+      <c r="H48" s="9"/>
+      <c r="I48" s="13"/>
       <c r="J48" s="8"/>
-      <c r="K48" s="8" t="s">
-        <v>170</v>
-      </c>
+      <c r="K48" s="5"/>
       <c r="L48" s="8"/>
     </row>
     <row r="49" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B49" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>13</v>
+      <c r="B49" s="10"/>
+      <c r="C49" s="9" t="s">
+        <v>12</v>
       </c>
       <c r="D49" s="6">
-        <v>45635</v>
+        <v>45632</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F49" s="8"/>
       <c r="G49" s="8"/>
       <c r="H49" s="8"/>
-      <c r="I49" s="8"/>
-      <c r="J49" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="K49" s="13" t="s">
+      <c r="I49" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="L49" s="8"/>
+    </row>
+    <row r="50" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B50" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D50" s="6">
+        <v>45635</v>
+      </c>
+      <c r="E50" s="7" t="s">
         <v>168</v>
-      </c>
-      <c r="L49" s="8"/>
-    </row>
-    <row r="50" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B50" s="4"/>
-      <c r="C50" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="D50" s="6">
-        <v>45636</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>174</v>
       </c>
       <c r="F50" s="8"/>
       <c r="G50" s="8"/>
       <c r="H50" s="8"/>
       <c r="I50" s="8"/>
-      <c r="J50" s="8" t="s">
-        <v>175</v>
-      </c>
-      <c r="K50" s="8" t="s">
-        <v>176</v>
+      <c r="J50" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="K50" s="13" t="s">
+        <v>168</v>
       </c>
       <c r="L50" s="8"/>
     </row>
-    <row r="51" spans="2:12" ht="66" x14ac:dyDescent="0.3">
-      <c r="B51" s="10"/>
+    <row r="51" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B51" s="4"/>
       <c r="C51" s="5" t="s">
-        <v>10</v>
+        <v>173</v>
       </c>
       <c r="D51" s="6">
-        <v>45637</v>
+        <v>45636</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F51" s="8"/>
       <c r="G51" s="8"/>
@@ -2776,15 +2794,38 @@
         <v>175</v>
       </c>
       <c r="K51" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="L51" s="8"/>
+    </row>
+    <row r="52" spans="2:12" ht="66" x14ac:dyDescent="0.3">
+      <c r="B52" s="10"/>
+      <c r="C52" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D52" s="6">
+        <v>45637</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="K52" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="L51" s="5" t="s">
+      <c r="L52" s="5" t="s">
         <v>33</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J16" r:id="rId1" location="project-proposal" display="https://mat212fa24.netlify.app/project-instructions#project-proposal" xr:uid="{640FB934-CEF3-4FA6-8044-3AEE5553F6A5}"/>
+    <hyperlink ref="J17" r:id="rId1" location="project-proposal" display="https://mat212fa24.netlify.app/project-instructions#project-proposal" xr:uid="{640FB934-CEF3-4FA6-8044-3AEE5553F6A5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Updated math models and added hw
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efriedlander\Dropbox\OneDrive - The College of Idaho\Teaching\MAT212WI25\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yotescollegeofidaho-my.sharepoint.com/personal/efriedlander_collegeofidaho_edu/Documents/Teaching/MAT212WI25/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A521D35A-ABFE-4B34-A838-A012BBCA88C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{A521D35A-ABFE-4B34-A838-A012BBCA88C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2ADF4398-1747-4F1A-95C6-AD901116F05D}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="203">
   <si>
     <t>dow</t>
   </si>
@@ -637,13 +637,19 @@
   </si>
   <si>
     <t>/ae/ae-04-math-models.qmd</t>
+  </si>
+  <si>
+    <t>T/W</t>
+  </si>
+  <si>
+    <t>/hw/hw-03.qmd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1163,7 +1169,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1183,10 +1189,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1508,16 +1510,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C666FC1-734D-4F31-9D28-5509B94BC597}">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.5">
+    <row r="1" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>34</v>
       </c>
@@ -1555,7 +1557,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="49.5">
+    <row r="2" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -1587,7 +1589,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="99">
+    <row r="3" spans="1:12" ht="99" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1621,7 +1623,7 @@
       <c r="K3" s="8"/>
       <c r="L3" s="5"/>
     </row>
-    <row r="4" spans="1:12" ht="82.5">
+    <row r="4" spans="1:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1629,7 +1631,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="D4" s="6">
         <v>45664</v>
@@ -1655,7 +1657,7 @@
       <c r="K4" s="8"/>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:12" ht="115.5">
+    <row r="5" spans="1:12" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -1680,14 +1682,16 @@
       <c r="H5" t="s">
         <v>200</v>
       </c>
-      <c r="I5" s="8"/>
+      <c r="I5" s="8" t="s">
+        <v>202</v>
+      </c>
       <c r="J5" s="8" t="s">
         <v>184</v>
       </c>
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
     </row>
-    <row r="6" spans="1:12" ht="66">
+    <row r="6" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B6" s="10"/>
       <c r="C6" s="5" t="s">
         <v>10</v>
@@ -1720,7 +1724,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="49.5">
+    <row r="7" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B7" s="10"/>
       <c r="C7" s="5" t="s">
         <v>12</v>
@@ -1745,7 +1749,7 @@
       <c r="K7" s="26"/>
       <c r="L7" s="12"/>
     </row>
-    <row r="8" spans="1:12" ht="16.5">
+    <row r="8" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B8" s="4">
         <v>3</v>
       </c>
@@ -1759,7 +1763,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="99">
+    <row r="9" spans="1:12" ht="115.5" x14ac:dyDescent="0.3">
       <c r="B9" s="4"/>
       <c r="C9" s="5" t="s">
         <v>10</v>
@@ -1788,7 +1792,7 @@
       </c>
       <c r="L9" s="8"/>
     </row>
-    <row r="10" spans="1:12" ht="165">
+    <row r="10" spans="1:12" ht="181.5" x14ac:dyDescent="0.3">
       <c r="B10" s="10"/>
       <c r="C10" s="5" t="s">
         <v>12</v>
@@ -1817,7 +1821,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="115.5">
+    <row r="11" spans="1:12" ht="115.5" x14ac:dyDescent="0.3">
       <c r="B11" s="4">
         <v>4</v>
       </c>
@@ -1842,7 +1846,7 @@
       <c r="K11" s="8"/>
       <c r="L11" s="8"/>
     </row>
-    <row r="12" spans="1:12" ht="148.5">
+    <row r="12" spans="1:12" ht="148.5" x14ac:dyDescent="0.3">
       <c r="B12" s="10"/>
       <c r="C12" s="5" t="s">
         <v>10</v>
@@ -1864,7 +1868,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="8"/>
     </row>
-    <row r="13" spans="1:12" ht="66">
+    <row r="13" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="5" t="s">
         <v>12</v>
@@ -1893,7 +1897,7 @@
       </c>
       <c r="L13" s="8"/>
     </row>
-    <row r="14" spans="1:12" ht="99">
+    <row r="14" spans="1:12" ht="99" x14ac:dyDescent="0.3">
       <c r="B14" s="30">
         <v>5</v>
       </c>
@@ -1920,7 +1924,7 @@
       <c r="K14" s="34"/>
       <c r="L14" s="33"/>
     </row>
-    <row r="15" spans="1:12" ht="66">
+    <row r="15" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B15" s="30"/>
       <c r="C15" s="31" t="s">
         <v>10</v>
@@ -1945,7 +1949,7 @@
       <c r="K15" s="34"/>
       <c r="L15" s="33"/>
     </row>
-    <row r="16" spans="1:12" ht="49.5">
+    <row r="16" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B16" s="30"/>
       <c r="C16" s="31" t="s">
         <v>12</v>
@@ -1974,7 +1978,7 @@
       </c>
       <c r="L16" s="33"/>
     </row>
-    <row r="17" spans="2:12" ht="49.5">
+    <row r="17" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B17" s="30">
         <v>6</v>
       </c>
@@ -2001,7 +2005,7 @@
       </c>
       <c r="L17" s="33"/>
     </row>
-    <row r="18" spans="2:12" ht="99">
+    <row r="18" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
       <c r="B18" s="30"/>
       <c r="C18" s="31" t="s">
         <v>10</v>
@@ -2017,7 +2021,7 @@
       <c r="K18" s="34"/>
       <c r="L18" s="33"/>
     </row>
-    <row r="19" spans="2:12" ht="33">
+    <row r="19" spans="2:12" ht="33" x14ac:dyDescent="0.3">
       <c r="B19" s="30"/>
       <c r="C19" s="31" t="s">
         <v>12</v>
@@ -2046,7 +2050,7 @@
       </c>
       <c r="L19" s="33"/>
     </row>
-    <row r="20" spans="2:12" ht="66">
+    <row r="20" spans="2:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B20" s="4">
         <v>7</v>
       </c>
@@ -2072,7 +2076,7 @@
       <c r="J20" s="22"/>
       <c r="L20" s="22"/>
     </row>
-    <row r="21" spans="2:12" ht="66">
+    <row r="21" spans="2:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B21" s="18"/>
       <c r="C21" s="40" t="s">
         <v>10</v>
@@ -2097,7 +2101,7 @@
       <c r="K21" s="23"/>
       <c r="L21" s="23"/>
     </row>
-    <row r="22" spans="2:12" ht="49.5">
+    <row r="22" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B22" s="10"/>
       <c r="C22" s="39" t="s">
         <v>12</v>
@@ -2126,7 +2130,7 @@
       </c>
       <c r="L22" s="8"/>
     </row>
-    <row r="23" spans="2:12" ht="66">
+    <row r="23" spans="2:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B23" s="4">
         <v>8</v>
       </c>
@@ -2153,7 +2157,7 @@
       <c r="K23" s="8"/>
       <c r="L23" s="8"/>
     </row>
-    <row r="24" spans="2:12" ht="33">
+    <row r="24" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B24" s="4"/>
       <c r="C24" s="5" t="s">
         <v>10</v>
@@ -2178,7 +2182,7 @@
       <c r="K24" s="5"/>
       <c r="L24" s="8"/>
     </row>
-    <row r="25" spans="2:12" ht="16.5">
+    <row r="25" spans="2:12" ht="33" x14ac:dyDescent="0.3">
       <c r="B25" s="10"/>
       <c r="C25" s="5" t="s">
         <v>12</v>
@@ -2199,7 +2203,7 @@
       </c>
       <c r="L25" s="8"/>
     </row>
-    <row r="26" spans="2:12" ht="66">
+    <row r="26" spans="2:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B26" s="4">
         <v>9</v>
       </c>
@@ -2222,7 +2226,7 @@
       </c>
       <c r="L26" s="8"/>
     </row>
-    <row r="27" spans="2:12" ht="66">
+    <row r="27" spans="2:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B27" s="10"/>
       <c r="C27" s="9" t="s">
         <v>10</v>
@@ -2241,7 +2245,7 @@
       <c r="K27" s="8"/>
       <c r="L27" s="8"/>
     </row>
-    <row r="28" spans="2:12" ht="66">
+    <row r="28" spans="2:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B28" s="4"/>
       <c r="C28" s="5" t="s">
         <v>12</v>
@@ -2260,7 +2264,7 @@
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
     </row>
-    <row r="29" spans="2:12" ht="49.5">
+    <row r="29" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B29" s="4">
         <v>10</v>
       </c>
@@ -2287,7 +2291,7 @@
       <c r="K29" s="8"/>
       <c r="L29" s="8"/>
     </row>
-    <row r="30" spans="2:12" ht="66">
+    <row r="30" spans="2:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B30" s="10"/>
       <c r="C30" s="9" t="s">
         <v>10</v>
@@ -2314,7 +2318,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="31" spans="2:12" ht="99">
+    <row r="31" spans="2:12" ht="99" x14ac:dyDescent="0.3">
       <c r="B31" s="4"/>
       <c r="C31" s="5" t="s">
         <v>12</v>
@@ -2341,7 +2345,7 @@
       </c>
       <c r="L31" s="8"/>
     </row>
-    <row r="32" spans="2:12" ht="49.5">
+    <row r="32" spans="2:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B32" s="4">
         <v>11</v>
       </c>
@@ -2368,7 +2372,7 @@
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
     </row>
-    <row r="33" spans="2:12" ht="49.5">
+    <row r="33" spans="2:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B33" s="10"/>
       <c r="C33" s="9" t="s">
         <v>10</v>
@@ -2397,7 +2401,7 @@
       </c>
       <c r="L33" s="46"/>
     </row>
-    <row r="34" spans="2:12" ht="82.5">
+    <row r="34" spans="2:12" ht="99" x14ac:dyDescent="0.3">
       <c r="B34" s="4"/>
       <c r="C34" s="5" t="s">
         <v>12</v>
@@ -2425,7 +2429,7 @@
       </c>
       <c r="L34" s="49"/>
     </row>
-    <row r="35" spans="2:12" ht="49.5">
+    <row r="35" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B35" s="4">
         <v>12</v>
       </c>
@@ -2452,7 +2456,7 @@
       <c r="K35" s="48"/>
       <c r="L35" s="47"/>
     </row>
-    <row r="36" spans="2:12" ht="82.5">
+    <row r="36" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="B36" s="10"/>
       <c r="C36" s="9" t="s">
         <v>10</v>
@@ -2477,7 +2481,7 @@
       <c r="K36" s="13"/>
       <c r="L36" s="8"/>
     </row>
-    <row r="37" spans="2:12" ht="82.5">
+    <row r="37" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="B37" s="4"/>
       <c r="C37" s="5" t="s">
         <v>12</v>
@@ -2503,7 +2507,7 @@
       </c>
       <c r="L37" s="8"/>
     </row>
-    <row r="38" spans="2:12" ht="82.5">
+    <row r="38" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="B38" s="4">
         <v>13</v>
       </c>
@@ -2528,7 +2532,7 @@
       <c r="K38" s="5"/>
       <c r="L38" s="8"/>
     </row>
-    <row r="39" spans="2:12" ht="82.5">
+    <row r="39" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="B39" s="10"/>
       <c r="C39" s="5" t="s">
         <v>10</v>
@@ -2553,7 +2557,7 @@
       <c r="K39" s="8"/>
       <c r="L39" s="8"/>
     </row>
-    <row r="40" spans="2:12" ht="115.5">
+    <row r="40" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
       <c r="B40" s="4"/>
       <c r="C40" s="5" t="s">
         <v>12</v>
@@ -2580,7 +2584,7 @@
       </c>
       <c r="L40" s="8"/>
     </row>
-    <row r="41" spans="2:12" ht="66">
+    <row r="41" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="B41" s="4">
         <v>14</v>
       </c>
@@ -2613,7 +2617,7 @@
       </c>
       <c r="L41" s="8"/>
     </row>
-    <row r="42" spans="2:12" ht="66">
+    <row r="42" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="B42" s="10"/>
       <c r="C42" s="9" t="s">
         <v>10</v>
@@ -2638,7 +2642,7 @@
       <c r="K42" s="8"/>
       <c r="L42" s="5"/>
     </row>
-    <row r="43" spans="2:12" ht="66">
+    <row r="43" spans="2:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="B43" s="4"/>
       <c r="C43" s="5" t="s">
         <v>12</v>
@@ -2663,7 +2667,7 @@
       <c r="K43" s="8"/>
       <c r="L43" s="8"/>
     </row>
-    <row r="44" spans="2:12" ht="33">
+    <row r="44" spans="2:12" ht="33" x14ac:dyDescent="0.3">
       <c r="B44" s="4">
         <v>15</v>
       </c>
@@ -2692,7 +2696,7 @@
       </c>
       <c r="L44" s="8"/>
     </row>
-    <row r="45" spans="2:12" ht="16.5">
+    <row r="45" spans="2:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B45" s="10"/>
       <c r="C45" s="9" t="s">
         <v>10</v>
@@ -2711,7 +2715,7 @@
       <c r="K45" s="13"/>
       <c r="L45" s="12"/>
     </row>
-    <row r="46" spans="2:12" ht="86.25" customHeight="1">
+    <row r="46" spans="2:12" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="10"/>
       <c r="C46" s="5" t="s">
         <v>12</v>
@@ -2730,7 +2734,7 @@
       <c r="K46" s="8"/>
       <c r="L46" s="8"/>
     </row>
-    <row r="47" spans="2:12" ht="99">
+    <row r="47" spans="2:12" ht="115.5" x14ac:dyDescent="0.3">
       <c r="B47" s="4">
         <v>16</v>
       </c>
@@ -2756,7 +2760,7 @@
       <c r="K47" s="8"/>
       <c r="L47" s="5"/>
     </row>
-    <row r="48" spans="2:12" ht="33">
+    <row r="48" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B48" s="10"/>
       <c r="C48" s="5" t="s">
         <v>10</v>
@@ -2775,7 +2779,7 @@
       <c r="K48" s="5"/>
       <c r="L48" s="8"/>
     </row>
-    <row r="49" spans="2:12" ht="33">
+    <row r="49" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B49" s="10"/>
       <c r="C49" s="9" t="s">
         <v>12</v>
@@ -2798,7 +2802,7 @@
       </c>
       <c r="L49" s="8"/>
     </row>
-    <row r="50" spans="2:12" ht="49.5">
+    <row r="50" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B50" s="4" t="s">
         <v>170</v>
       </c>
@@ -2823,7 +2827,7 @@
       </c>
       <c r="L50" s="8"/>
     </row>
-    <row r="51" spans="2:12" ht="49.5">
+    <row r="51" spans="2:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B51" s="4"/>
       <c r="C51" s="5" t="s">
         <v>171</v>
@@ -2846,7 +2850,7 @@
       </c>
       <c r="L51" s="8"/>
     </row>
-    <row r="52" spans="2:12" ht="66">
+    <row r="52" spans="2:12" ht="66" x14ac:dyDescent="0.3">
       <c r="B52" s="10"/>
       <c r="C52" s="5" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Updated schedule and prep
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efriedlander\Dropbox\OneDrive - The College of Idaho\Teaching\MAT212WI25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53946E8C-8714-4ADB-B689-6AA6559229CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3861F29-B60B-416D-A24B-560DA896E329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="198">
   <si>
     <t>dow</t>
   </si>
@@ -621,10 +621,13 @@
     <t>TH</t>
   </si>
   <si>
-    <t>SLR: Conditions and Evaluation</t>
-  </si>
-  <si>
     <t>/prepare/prep-05.qmd</t>
+  </si>
+  <si>
+    <t>T/W</t>
+  </si>
+  <si>
+    <t>SLR: Conditions</t>
   </si>
 </sst>
 </file>
@@ -1497,7 +1500,7 @@
   <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -1617,7 +1620,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>164</v>
+        <v>196</v>
       </c>
       <c r="D4" s="6">
         <v>45664</v>
@@ -1675,7 +1678,7 @@
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
     </row>
-    <row r="6" spans="1:12" ht="82.5">
+    <row r="6" spans="1:12" ht="49.5">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -1689,10 +1692,10 @@
         <v>45666</v>
       </c>
       <c r="E6" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="F6" s="51" t="s">
         <v>195</v>
-      </c>
-      <c r="F6" s="51" t="s">
-        <v>196</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="9"/>

</xml_diff>

<commit_message>
Updated hw 3 and schedule
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efriedlander\Dropbox\OneDrive - The College of Idaho\Teaching\MAT212WI25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4B4EE7-B5CE-4CEB-890F-15A3864D52AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D800D64F-9A5B-4655-B5B2-8D0882A3C766}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
   </bookViews>
@@ -1157,7 +1157,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1177,10 +1177,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1502,8 +1498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C666FC1-734D-4F31-9D28-5509B94BC597}">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:I7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -1657,7 +1653,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>10</v>
+        <v>192</v>
       </c>
       <c r="D5" s="6">
         <v>45665</v>
@@ -1701,6 +1697,15 @@
       </c>
       <c r="F6" s="51" t="s">
         <v>193</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="H6" t="s">
+        <v>198</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>197</v>
       </c>
       <c r="J6" s="8" t="s">
         <v>176</v>
@@ -1720,15 +1725,6 @@
         <v>32</v>
       </c>
       <c r="F7" s="5"/>
-      <c r="G7" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="H7" t="s">
-        <v>198</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>197</v>
-      </c>
       <c r="J7" s="8" t="s">
         <v>176</v>
       </c>

</xml_diff>

<commit_message>
Reorganizing lectures and added eval
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efriedlander\Dropbox\OneDrive - The College of Idaho\Teaching\MAT212WI25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{793480F6-7377-465F-9A4F-6C7B2B4164DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB977B32-59E8-4069-888F-A7ACA7A65E1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="201">
   <si>
     <t>dow</t>
   </si>
@@ -615,9 +615,6 @@
     <t>T/W</t>
   </si>
   <si>
-    <t>SLR: Conditions</t>
-  </si>
-  <si>
     <t>/slides/05-slr-conditions.qmd</t>
   </si>
   <si>
@@ -627,9 +624,6 @@
     <t>/ae/ae-05-conditions.qmd</t>
   </si>
   <si>
-    <t>Model Evaluation</t>
-  </si>
-  <si>
     <t>/prepare/prep-06.qmd</t>
   </si>
   <si>
@@ -640,6 +634,9 @@
   </si>
   <si>
     <t>/project/project-instructions.qmd#load-data</t>
+  </si>
+  <si>
+    <t>SLR: Conditions + Evaluation</t>
   </si>
 </sst>
 </file>
@@ -1168,8 +1165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C666FC1-734D-4F31-9D28-5509B94BC597}">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -1341,7 +1338,7 @@
         <v>189</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>173</v>
@@ -1349,7 +1346,7 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" ht="49.5">
+    <row r="6" spans="1:12" ht="82.5">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -1357,25 +1354,25 @@
         <v>5</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>190</v>
+        <v>11</v>
       </c>
       <c r="D6" s="8">
         <v>45666</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>191</v>
       </c>
       <c r="G6" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>174</v>
@@ -1383,7 +1380,7 @@
       <c r="K6" s="1"/>
       <c r="L6" s="11"/>
     </row>
-    <row r="7" spans="1:12" ht="49.5">
+    <row r="7" spans="1:12" ht="16.5">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -1391,44 +1388,40 @@
         <v>6</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7" s="8">
         <v>45667</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="12" t="s">
         <v>197</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="G7" s="5"/>
+        <v>196</v>
+      </c>
+      <c r="G7" s="7"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="11"/>
     </row>
     <row r="8" spans="1:12" ht="16.5">
-      <c r="A8" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="A8" s="5"/>
       <c r="B8" s="6">
         <v>7</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>181</v>
-      </c>
+      <c r="C8" s="7"/>
       <c r="D8" s="8">
         <v>45667</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>

</xml_diff>

<commit_message>
Added transformation and outliers
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efriedlander\Dropbox\OneDrive - The College of Idaho\Teaching\MAT212WI25\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yotescollegeofidaho-my.sharepoint.com/personal/efriedlander_collegeofidaho_edu/Documents/Teaching/MAT212WI25/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1953B0-C58F-4BC7-8266-F6592DEE9EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{6D1953B0-C58F-4BC7-8266-F6592DEE9EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8496C45B-0D88-4DB0-8526-278B2ED7757C}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="206">
   <si>
     <t>dow</t>
   </si>
@@ -639,14 +639,26 @@
     <t>SLR: Conditions + Evaluation</t>
   </si>
   <si>
-    <t>Multiple Linear Regression</t>
+    <t>/slides/06-slr-transformations.qmd</t>
+  </si>
+  <si>
+    <t>/ae/ae-06-transformations.qmd</t>
+  </si>
+  <si>
+    <t>/hw/hw-04.qmd</t>
+  </si>
+  <si>
+    <t>/project/project-instructions.qmd#plots-tables</t>
+  </si>
+  <si>
+    <t>Intro to Multiple Linear Regression</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -847,6 +859,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1169,15 +1185,15 @@
   <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="16.5">
+    <row r="1" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -1215,7 +1231,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="49.5">
+    <row r="2" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>30</v>
       </c>
@@ -1247,7 +1263,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="99">
+    <row r="3" spans="1:12" ht="99" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>30</v>
       </c>
@@ -1281,7 +1297,7 @@
       <c r="K3" s="1"/>
       <c r="L3" s="7"/>
     </row>
-    <row r="4" spans="1:12" ht="82.5">
+    <row r="4" spans="1:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>30</v>
       </c>
@@ -1315,7 +1331,7 @@
       <c r="K4" s="1"/>
       <c r="L4" s="7"/>
     </row>
-    <row r="5" spans="1:12" ht="115.5">
+    <row r="5" spans="1:12" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>30</v>
       </c>
@@ -1349,7 +1365,7 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" ht="82.5">
+    <row r="6" spans="1:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>30</v>
       </c>
@@ -1357,7 +1373,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>11</v>
+        <v>181</v>
       </c>
       <c r="D6" s="8">
         <v>45666</v>
@@ -1383,7 +1399,7 @@
       <c r="K6" s="1"/>
       <c r="L6" s="11"/>
     </row>
-    <row r="7" spans="1:12" ht="16.5">
+    <row r="7" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>30</v>
       </c>
@@ -1402,16 +1418,22 @@
       <c r="F7" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+      <c r="G7" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>203</v>
+      </c>
       <c r="J7" s="1" t="s">
         <v>199</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="11"/>
     </row>
-    <row r="8" spans="1:12" ht="16.5">
+    <row r="8" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>30</v>
       </c>
@@ -1419,13 +1441,13 @@
         <v>7</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>12</v>
+        <v>160</v>
       </c>
       <c r="D8" s="8">
-        <v>45667</v>
+        <v>45668</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>198</v>
@@ -1433,11 +1455,13 @@
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
+      <c r="J8" s="1" t="s">
+        <v>204</v>
+      </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" ht="99">
+    <row r="9" spans="1:12" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
       <c r="C9" s="7" t="s">
@@ -1467,7 +1491,7 @@
       </c>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" ht="165">
+    <row r="10" spans="1:12" ht="181.5" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="14"/>
       <c r="C10" s="7" t="s">
@@ -1497,7 +1521,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="115.5">
+    <row r="11" spans="1:12" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="6">
         <v>4</v>
@@ -1523,7 +1547,7 @@
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" ht="148.5">
+    <row r="12" spans="1:12" ht="148.5" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
       <c r="B12" s="14"/>
       <c r="C12" s="7" t="s">
@@ -1547,7 +1571,7 @@
       <c r="K12" s="7"/>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12" ht="66">
+    <row r="13" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="6"/>
       <c r="C13" s="7" t="s">
@@ -1577,7 +1601,7 @@
       </c>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:12" ht="99">
+    <row r="14" spans="1:12" ht="99" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
       <c r="B14" s="6">
         <v>5</v>
@@ -1605,7 +1629,7 @@
       <c r="K14" s="7"/>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" ht="66">
+    <row r="15" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="7" t="s">
@@ -1631,7 +1655,7 @@
       <c r="K15" s="7"/>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12" ht="49.5">
+    <row r="16" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="7" t="s">
@@ -1661,7 +1685,7 @@
       </c>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:12" ht="49.5">
+    <row r="17" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="6">
         <v>6</v>
@@ -1689,7 +1713,7 @@
       </c>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12" ht="99">
+    <row r="18" spans="1:12" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="7" t="s">
@@ -1709,7 +1733,7 @@
       <c r="K18" s="7"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12" ht="33">
+    <row r="19" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7" t="s">
@@ -1739,7 +1763,7 @@
       </c>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:12" ht="66">
+    <row r="20" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A20" s="5"/>
       <c r="B20" s="6">
         <v>7</v>
@@ -1767,7 +1791,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12" ht="66">
+    <row r="21" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
       <c r="B21" s="14"/>
       <c r="C21" s="13" t="s">
@@ -1793,7 +1817,7 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" ht="49.5">
+    <row r="22" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
       <c r="B22" s="14"/>
       <c r="C22" s="13" t="s">
@@ -1823,7 +1847,7 @@
       </c>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" ht="66">
+    <row r="23" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A23" s="5"/>
       <c r="B23" s="6">
         <v>8</v>
@@ -1851,7 +1875,7 @@
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="1:12" ht="33">
+    <row r="24" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A24" s="5"/>
       <c r="B24" s="6"/>
       <c r="C24" s="7" t="s">
@@ -1877,7 +1901,7 @@
       <c r="K24" s="7"/>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12" ht="16.5">
+    <row r="25" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
       <c r="B25" s="14"/>
       <c r="C25" s="7" t="s">
@@ -1899,7 +1923,7 @@
       </c>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="1:12" ht="66">
+    <row r="26" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
       <c r="B26" s="6">
         <v>9</v>
@@ -1923,7 +1947,7 @@
       </c>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:12" ht="66">
+    <row r="27" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
       <c r="B27" s="14"/>
       <c r="C27" s="7" t="s">
@@ -1943,7 +1967,7 @@
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
     </row>
-    <row r="28" spans="1:12" ht="66">
+    <row r="28" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A28" s="5"/>
       <c r="B28" s="6"/>
       <c r="C28" s="7" t="s">
@@ -1963,7 +1987,7 @@
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
     </row>
-    <row r="29" spans="1:12" ht="49.5">
+    <row r="29" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A29" s="5"/>
       <c r="B29" s="6">
         <v>10</v>
@@ -1991,7 +2015,7 @@
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
     </row>
-    <row r="30" spans="1:12" ht="66">
+    <row r="30" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A30" s="5"/>
       <c r="B30" s="14"/>
       <c r="C30" s="7" t="s">
@@ -2019,7 +2043,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="99">
+    <row r="31" spans="1:12" ht="99" x14ac:dyDescent="0.3">
       <c r="A31" s="5"/>
       <c r="B31" s="6"/>
       <c r="C31" s="7" t="s">
@@ -2047,7 +2071,7 @@
       </c>
       <c r="L31" s="1"/>
     </row>
-    <row r="32" spans="1:12" ht="49.5">
+    <row r="32" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A32" s="5"/>
       <c r="B32" s="6">
         <v>11</v>
@@ -2075,7 +2099,7 @@
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" spans="1:12" ht="49.5">
+    <row r="33" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A33" s="5"/>
       <c r="B33" s="14"/>
       <c r="C33" s="7" t="s">
@@ -2105,7 +2129,7 @@
       </c>
       <c r="L33" s="1"/>
     </row>
-    <row r="34" spans="1:12" ht="82.5">
+    <row r="34" spans="1:12" ht="99" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
       <c r="B34" s="6"/>
       <c r="C34" s="7" t="s">
@@ -2135,7 +2159,7 @@
       </c>
       <c r="L34" s="1"/>
     </row>
-    <row r="35" spans="1:12" ht="49.5">
+    <row r="35" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
       <c r="B35" s="6">
         <v>12</v>
@@ -2163,7 +2187,7 @@
       <c r="K35" s="7"/>
       <c r="L35" s="1"/>
     </row>
-    <row r="36" spans="1:12" ht="82.5">
+    <row r="36" spans="1:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A36" s="5"/>
       <c r="B36" s="14"/>
       <c r="C36" s="7" t="s">
@@ -2189,7 +2213,7 @@
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
     </row>
-    <row r="37" spans="1:12" ht="82.5">
+    <row r="37" spans="1:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A37" s="5"/>
       <c r="B37" s="6"/>
       <c r="C37" s="7" t="s">
@@ -2217,7 +2241,7 @@
       </c>
       <c r="L37" s="1"/>
     </row>
-    <row r="38" spans="1:12" ht="82.5">
+    <row r="38" spans="1:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A38" s="5"/>
       <c r="B38" s="6">
         <v>13</v>
@@ -2243,7 +2267,7 @@
       <c r="K38" s="7"/>
       <c r="L38" s="1"/>
     </row>
-    <row r="39" spans="1:12" ht="82.5">
+    <row r="39" spans="1:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A39" s="5"/>
       <c r="B39" s="14"/>
       <c r="C39" s="7" t="s">
@@ -2269,7 +2293,7 @@
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
     </row>
-    <row r="40" spans="1:12" ht="115.5">
+    <row r="40" spans="1:12" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A40" s="5"/>
       <c r="B40" s="6"/>
       <c r="C40" s="7" t="s">
@@ -2297,7 +2321,7 @@
       </c>
       <c r="L40" s="1"/>
     </row>
-    <row r="41" spans="1:12" ht="66">
+    <row r="41" spans="1:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A41" s="5"/>
       <c r="B41" s="6">
         <v>14</v>
@@ -2331,7 +2355,7 @@
       </c>
       <c r="L41" s="1"/>
     </row>
-    <row r="42" spans="1:12" ht="66">
+    <row r="42" spans="1:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A42" s="5"/>
       <c r="B42" s="14"/>
       <c r="C42" s="7" t="s">
@@ -2357,7 +2381,7 @@
       <c r="K42" s="1"/>
       <c r="L42" s="7"/>
     </row>
-    <row r="43" spans="1:12" ht="66">
+    <row r="43" spans="1:12" ht="82.5" x14ac:dyDescent="0.3">
       <c r="A43" s="5"/>
       <c r="B43" s="6"/>
       <c r="C43" s="7" t="s">
@@ -2383,7 +2407,7 @@
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
     </row>
-    <row r="44" spans="1:12" ht="33">
+    <row r="44" spans="1:12" ht="33" x14ac:dyDescent="0.3">
       <c r="A44" s="5"/>
       <c r="B44" s="6">
         <v>15</v>
@@ -2413,7 +2437,7 @@
       </c>
       <c r="L44" s="1"/>
     </row>
-    <row r="45" spans="1:12" ht="16.5">
+    <row r="45" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A45" s="5"/>
       <c r="B45" s="14"/>
       <c r="C45" s="7" t="s">
@@ -2433,7 +2457,7 @@
       <c r="K45" s="1"/>
       <c r="L45" s="11"/>
     </row>
-    <row r="46" spans="1:12" ht="86.25" customHeight="1">
+    <row r="46" spans="1:12" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5"/>
       <c r="B46" s="14"/>
       <c r="C46" s="7" t="s">
@@ -2453,7 +2477,7 @@
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
     </row>
-    <row r="47" spans="1:12" ht="99">
+    <row r="47" spans="1:12" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A47" s="5"/>
       <c r="B47" s="6">
         <v>16</v>
@@ -2481,7 +2505,7 @@
       <c r="K47" s="1"/>
       <c r="L47" s="7"/>
     </row>
-    <row r="48" spans="1:12" ht="33">
+    <row r="48" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A48" s="5"/>
       <c r="B48" s="14"/>
       <c r="C48" s="7" t="s">
@@ -2501,7 +2525,7 @@
       <c r="K48" s="7"/>
       <c r="L48" s="1"/>
     </row>
-    <row r="49" spans="1:12" ht="33">
+    <row r="49" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A49" s="5"/>
       <c r="B49" s="14"/>
       <c r="C49" s="7" t="s">
@@ -2525,7 +2549,7 @@
       </c>
       <c r="L49" s="1"/>
     </row>
-    <row r="50" spans="1:12" ht="49.5">
+    <row r="50" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A50" s="5"/>
       <c r="B50" s="6" t="s">
         <v>159</v>
@@ -2551,7 +2575,7 @@
       </c>
       <c r="L50" s="1"/>
     </row>
-    <row r="51" spans="1:12" ht="49.5">
+    <row r="51" spans="1:12" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A51" s="5"/>
       <c r="B51" s="6"/>
       <c r="C51" s="7" t="s">
@@ -2575,7 +2599,7 @@
       </c>
       <c r="L51" s="1"/>
     </row>
-    <row r="52" spans="1:12" ht="66">
+    <row r="52" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A52" s="5"/>
       <c r="B52" s="14"/>
       <c r="C52" s="7" t="s">

</xml_diff>

<commit_message>
Added logistic regression slides
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efriedlander\Dropbox\OneDrive - The College of Idaho\Teaching\MAT212WI25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291285C9-DD12-453E-925F-DD468ABD5938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D498EE-73FF-4461-9B5B-107F2C0FFB2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="203">
   <si>
     <t>dow</t>
   </si>
@@ -637,6 +637,12 @@
   </si>
   <si>
     <t>Introduction to Logistic Regression</t>
+  </si>
+  <si>
+    <t>/slides/09-logistic-intro.qmd</t>
+  </si>
+  <si>
+    <t>/ae/ae-09-logistic-intro.qmd</t>
   </si>
 </sst>
 </file>
@@ -1166,7 +1172,7 @@
   <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -1499,8 +1505,12 @@
       <c r="F10" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
+      <c r="G10" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>202</v>
+      </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1" t="s">
         <v>190</v>

</xml_diff>

<commit_message>
Added reading for next week
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efriedlander\Dropbox\OneDrive - The College of Idaho\Teaching\MAT212WI25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D498EE-73FF-4461-9B5B-107F2C0FFB2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6D4503-1EEE-4336-8AD6-D37223D29C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="205">
   <si>
     <t>dow</t>
   </si>
@@ -643,6 +643,12 @@
   </si>
   <si>
     <t>/ae/ae-09-logistic-intro.qmd</t>
+  </si>
+  <si>
+    <t>Logistic Regression: Inference</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1172,7 +1178,7 @@
   <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -1519,31 +1525,29 @@
       <c r="L10" s="7"/>
     </row>
     <row r="11" spans="1:12" ht="82.5">
-      <c r="A11" s="5"/>
+      <c r="A11" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="B11" s="6">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>199</v>
+        <v>139</v>
       </c>
       <c r="D11" s="8">
-        <v>45672</v>
+        <v>45677</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>193</v>
-      </c>
+        <v>204</v>
+      </c>
+      <c r="H11" s="7"/>
+      <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>

</xml_diff>

<commit_message>
Added logistic regression hw
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efriedlander\Dropbox\OneDrive - The College of Idaho\Teaching\MAT212WI25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6D4503-1EEE-4336-8AD6-D37223D29C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7EF87D-BBC5-4508-A71A-FBAD2C0D9C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="206">
   <si>
     <t>dow</t>
   </si>
@@ -649,6 +649,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>/hw/hw-07.qmd</t>
   </si>
 </sst>
 </file>
@@ -1178,7 +1181,7 @@
   <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -1517,7 +1520,9 @@
       <c r="H10" s="7" t="s">
         <v>202</v>
       </c>
-      <c r="I10" s="1"/>
+      <c r="I10" s="1" t="s">
+        <v>205</v>
+      </c>
       <c r="J10" s="1" t="s">
         <v>190</v>
       </c>

</xml_diff>

<commit_message>
Added logistic regression inference
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\efriedlander\Dropbox\OneDrive - The College of Idaho\Teaching\MAT212WI25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7EF87D-BBC5-4508-A71A-FBAD2C0D9C4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BF9106-F316-4A12-B964-CD09489FED9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="207">
   <si>
     <t>dow</t>
   </si>
@@ -111,9 +111,6 @@
     <t>x</t>
   </si>
   <si>
-    <t>SLR: Mathematical models for inference continued</t>
-  </si>
-  <si>
     <t>/ae/ae-05-math-models.html</t>
   </si>
   <si>
@@ -648,10 +645,16 @@
     <t>Logistic Regression: Inference</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>/hw/hw-07.qmd</t>
+  </si>
+  <si>
+    <t>Logistic</t>
+  </si>
+  <si>
+    <t>/slides/10-logistic-estimation-inference.qmd</t>
+  </si>
+  <si>
+    <t>/ae/ae-10-logistic-inference.qmd</t>
   </si>
 </sst>
 </file>
@@ -1180,8 +1183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C666FC1-734D-4F31-9D28-5509B94BC597}">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -1194,7 +1197,7 @@
         <v>23</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -1235,24 +1238,24 @@
         <v>1</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D2" s="8">
         <v>45660</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I2" s="10"/>
       <c r="J2" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K2" s="1"/>
       <c r="L2" s="7"/>
@@ -1265,28 +1268,28 @@
         <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D3" s="8">
         <v>45663</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K3" s="1"/>
       <c r="L3" s="7"/>
@@ -1299,28 +1302,28 @@
         <v>3</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D4" s="8">
         <v>45664</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G4" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="H4" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="J4" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K4" s="1"/>
       <c r="L4" s="7"/>
@@ -1333,7 +1336,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D5" s="8">
         <v>45666</v>
@@ -1342,19 +1345,19 @@
         <v>13</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G5" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="H5" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>168</v>
-      </c>
       <c r="I5" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -1367,28 +1370,28 @@
         <v>5</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D6" s="8">
         <v>45667</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G6" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>173</v>
-      </c>
       <c r="J6" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="11"/>
@@ -1407,22 +1410,22 @@
         <v>45670</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G7" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="I7" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>182</v>
-      </c>
       <c r="J7" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="11"/>
@@ -1435,28 +1438,28 @@
         <v>7</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D8" s="8">
         <v>45671</v>
       </c>
       <c r="E8" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="G8" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="G8" s="5" t="s">
+      <c r="H8" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="I8" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="I8" s="5" t="s">
-        <v>187</v>
-      </c>
       <c r="J8" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1469,28 +1472,28 @@
         <v>8</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D9" s="8">
         <v>45672</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="J9" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="K9" s="5"/>
       <c r="L9" s="1"/>
@@ -1509,22 +1512,22 @@
         <v>45673</v>
       </c>
       <c r="E10" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="G10" s="7" t="s">
+      <c r="H10" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="H10" s="7" t="s">
-        <v>202</v>
-      </c>
       <c r="I10" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="K10" s="7"/>
       <c r="L10" s="7"/>
@@ -1537,44 +1540,48 @@
         <v>10</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D11" s="8">
-        <v>45677</v>
+        <v>45678</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="H11" s="7"/>
+        <v>205</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>206</v>
+      </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" ht="148.5">
+    <row r="12" spans="1:12" ht="16.5">
       <c r="A12" s="5"/>
-      <c r="B12" s="14"/>
+      <c r="B12" s="6">
+        <v>11</v>
+      </c>
       <c r="C12" s="7" t="s">
         <v>10</v>
       </c>
       <c r="D12" s="8">
-        <v>45546</v>
+        <v>45679</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>25</v>
+        <v>204</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="1"/>
@@ -1587,25 +1594,25 @@
         <v>9</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D13" s="8">
         <v>45673</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
       <c r="J13" s="1"/>
       <c r="K13" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L13" s="1"/>
     </row>
@@ -1615,20 +1622,20 @@
         <v>10</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D14" s="8">
         <v>45673</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G14" s="7"/>
       <c r="H14" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -1645,16 +1652,16 @@
         <v>45553</v>
       </c>
       <c r="E15" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="7" t="s">
+      <c r="H15" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>32</v>
       </c>
       <c r="I15" s="9"/>
       <c r="J15" s="1"/>
@@ -1671,23 +1678,23 @@
         <v>45555</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I16" s="9" t="s">
         <v>18</v>
       </c>
       <c r="J16" s="1"/>
       <c r="K16" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L16" s="1"/>
     </row>
@@ -1703,10 +1710,10 @@
         <v>45558</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
@@ -1715,7 +1722,7 @@
         <v>16</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L17" s="1"/>
     </row>
@@ -1729,7 +1736,7 @@
         <v>45560</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
@@ -1749,23 +1756,23 @@
         <v>45562</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I19" s="9" t="s">
         <v>20</v>
       </c>
       <c r="J19" s="1"/>
       <c r="K19" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L19" s="1"/>
     </row>
@@ -1781,16 +1788,16 @@
         <v>45565</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -1807,16 +1814,16 @@
         <v>45567</v>
       </c>
       <c r="E21" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>53</v>
-      </c>
       <c r="H21" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
@@ -1833,23 +1840,23 @@
         <v>45569</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F22" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G22" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H22" s="1" t="s">
-        <v>56</v>
-      </c>
       <c r="I22" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L22" s="1"/>
     </row>
@@ -1865,16 +1872,16 @@
         <v>45572</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G23" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="I23" s="7"/>
       <c r="J23" s="1"/>
@@ -1894,13 +1901,13 @@
         <v>14</v>
       </c>
       <c r="F24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G24" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="G24" s="7" t="s">
-        <v>68</v>
-      </c>
       <c r="H24" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I24" s="7"/>
       <c r="J24" s="1"/>
@@ -1925,7 +1932,7 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L25" s="1"/>
     </row>
@@ -1941,7 +1948,7 @@
         <v>45579</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
@@ -1949,7 +1956,7 @@
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L26" s="1"/>
     </row>
@@ -1963,7 +1970,7 @@
         <v>45581</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
@@ -1983,7 +1990,7 @@
         <v>45583</v>
       </c>
       <c r="E28" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
@@ -2005,16 +2012,16 @@
         <v>45586</v>
       </c>
       <c r="E29" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G29" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F29" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="G29" s="7" t="s">
+      <c r="H29" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>71</v>
       </c>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
@@ -2031,22 +2038,22 @@
         <v>45588</v>
       </c>
       <c r="E30" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G30" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F30" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G30" s="7" t="s">
+      <c r="H30" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>74</v>
       </c>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="99">
@@ -2059,21 +2066,21 @@
         <v>45590</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="H31" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="H31" s="7" t="s">
-        <v>78</v>
-      </c>
       <c r="I31" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J31" s="1"/>
       <c r="K31" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L31" s="1"/>
     </row>
@@ -2089,16 +2096,16 @@
         <v>45593</v>
       </c>
       <c r="E32" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="F32" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="F32" s="7" t="s">
+      <c r="G32" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="G32" s="7" t="s">
+      <c r="H32" s="7" t="s">
         <v>87</v>
-      </c>
-      <c r="H32" s="7" t="s">
-        <v>88</v>
       </c>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -2115,23 +2122,23 @@
         <v>45595</v>
       </c>
       <c r="E33" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="G33" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="F33" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="G33" s="7" t="s">
+      <c r="H33" s="7" t="s">
         <v>91</v>
-      </c>
-      <c r="H33" s="7" t="s">
-        <v>92</v>
       </c>
       <c r="I33" s="1"/>
       <c r="J33" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="K33" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="K33" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="L33" s="1"/>
     </row>
@@ -2145,23 +2152,23 @@
         <v>45597</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G34" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="H34" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="H34" s="7" t="s">
-        <v>92</v>
-      </c>
       <c r="I34" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J34" s="5"/>
       <c r="K34" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L34" s="1"/>
     </row>
@@ -2180,13 +2187,13 @@
         <v>17</v>
       </c>
       <c r="F35" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G35" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="G35" s="7" t="s">
+      <c r="H35" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>95</v>
       </c>
       <c r="I35" s="7"/>
       <c r="J35" s="1"/>
@@ -2203,16 +2210,16 @@
         <v>45602</v>
       </c>
       <c r="E36" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G36" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="H36" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="H36" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="I36" s="1"/>
       <c r="J36" s="7"/>
@@ -2229,21 +2236,21 @@
         <v>45604</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F37" s="5"/>
       <c r="G37" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H37" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="I37" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="I37" s="7" t="s">
-        <v>104</v>
       </c>
       <c r="J37" s="1"/>
       <c r="K37" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L37" s="1"/>
     </row>
@@ -2259,13 +2266,13 @@
         <v>45607</v>
       </c>
       <c r="E38" s="9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G38" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H38" s="7"/>
       <c r="I38" s="1"/>
@@ -2286,13 +2293,13 @@
         <v>19</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
@@ -2309,21 +2316,21 @@
         <v>45611</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G40" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="H40" s="7" t="s">
         <v>111</v>
-      </c>
-      <c r="H40" s="7" t="s">
-        <v>112</v>
       </c>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L40" s="1"/>
     </row>
@@ -2339,25 +2346,25 @@
         <v>45614</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G41" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H41" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="H41" s="7" t="s">
-        <v>120</v>
-      </c>
       <c r="I41" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="J41" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K41" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L41" s="1"/>
     </row>
@@ -2371,16 +2378,16 @@
         <v>45616</v>
       </c>
       <c r="E42" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G42" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H42" s="7" t="s">
         <v>119</v>
-      </c>
-      <c r="H42" s="7" t="s">
-        <v>120</v>
       </c>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
@@ -2397,16 +2404,16 @@
         <v>45618</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G43" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H43" s="7" t="s">
         <v>119</v>
-      </c>
-      <c r="H43" s="7" t="s">
-        <v>120</v>
       </c>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
@@ -2425,21 +2432,21 @@
         <v>45621</v>
       </c>
       <c r="E44" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F44" s="1"/>
       <c r="G44" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H44" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I44" s="1"/>
       <c r="J44" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K44" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="L44" s="1"/>
     </row>
@@ -2453,7 +2460,7 @@
         <v>45623</v>
       </c>
       <c r="E45" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
@@ -2495,16 +2502,16 @@
         <v>45628</v>
       </c>
       <c r="E47" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="I47" s="1"/>
       <c r="J47" s="5"/>
@@ -2521,7 +2528,7 @@
         <v>45630</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F48" s="1"/>
       <c r="G48" s="7"/>
@@ -2541,24 +2548,24 @@
         <v>45632</v>
       </c>
       <c r="E49" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
       <c r="I49" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J49" s="1"/>
       <c r="K49" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="L49" s="1"/>
     </row>
     <row r="50" spans="1:12" ht="49.5">
       <c r="A50" s="5"/>
       <c r="B50" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>12</v>
@@ -2567,17 +2574,17 @@
         <v>45635</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
       <c r="J50" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K50" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L50" s="1"/>
     </row>
@@ -2585,23 +2592,23 @@
       <c r="A51" s="5"/>
       <c r="B51" s="6"/>
       <c r="C51" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D51" s="8">
         <v>45636</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
       <c r="J51" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="K51" s="1" t="s">
         <v>141</v>
-      </c>
-      <c r="K51" s="1" t="s">
-        <v>142</v>
       </c>
       <c r="L51" s="1"/>
     </row>
@@ -2615,17 +2622,17 @@
         <v>45637</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
       <c r="J52" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="L52" s="7" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
Add new course materials and update project documentation for MATH 2025
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricF\Documents\Teaching\MATH2025FA25\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA854B6E-1A69-4FF8-9DBB-CE8131922C5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D818CE0A-7F12-4407-94F9-528E0A7667BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{82B2C154-7672-424B-83B7-3BF61C3BA031}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>dow</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>lecture</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>Welcome to MATH 2025!</t>
   </si>
 </sst>
 </file>
@@ -602,7 +608,7 @@
   <dimension ref="A1:L53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,14 +654,22 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="16.5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="66" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9"/>
+      <c r="B2" s="6">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="8">
+        <v>45896</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="F2" s="1"/>
       <c r="G2" s="7"/>
       <c r="H2" s="5"/>

</xml_diff>